<commit_message>
write to  excel changes
</commit_message>
<xml_diff>
--- a/convertcsv.xlsx
+++ b/convertcsv.xlsx
@@ -2,10 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" r:id="rId1" sheetId="1"/>
   </sheets>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -40,16 +47,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -58,10 +65,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -215,7 +222,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -224,13 +231,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -240,7 +247,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -249,7 +256,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -258,7 +265,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -268,12 +275,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -304,7 +311,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -323,7 +330,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -375,7 +382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>

</xml_diff>